<commit_message>
Corrected text splitting into chunks and added alternative !not-yet-functional! topical chunker
</commit_message>
<xml_diff>
--- a/sentiment_comparison_reports.xlsx
+++ b/sentiment_comparison_reports.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CSRD Terms</t>
+          <t>CSRD Seeds</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>CSRD Reprasentative Words</t>
+          <t>CSRD Reprasentative Terms</t>
         </is>
       </c>
     </row>
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.74</v>
+        <v>3.66</v>
       </c>
       <c r="C2" t="n">
         <v>92</v>
@@ -478,7 +478,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.79</v>
+        <v>3.81</v>
       </c>
       <c r="C3" t="n">
         <v>285</v>
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.63</v>
+        <v>3.85</v>
       </c>
       <c r="C4" t="n">
         <v>351</v>
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.57</v>
+        <v>3.71</v>
       </c>
       <c r="C5" t="n">
         <v>427</v>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.37</v>
+        <v>3.55</v>
       </c>
       <c r="C6" t="n">
         <v>252</v>

</xml_diff>